<commit_message>
mejoras de clientes: dialog, plantillas, emailjs
</commit_message>
<xml_diff>
--- a/public/database/Clientes.xlsx
+++ b/public/database/Clientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio Aguilera\Desktop\Trabajo (SPA)\ProyectoReact\public\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF9FEA3-92A0-4F80-89C7-921B843F937E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6EF00B-7E6F-44AC-B02A-2A87603AE62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8880" xr2:uid="{D68F4056-0D45-4BC6-8B04-16C26C5398A7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D68F4056-0D45-4BC6-8B04-16C26C5398A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuarios" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>idCliente</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>Maivelynn@gmail.com</t>
+  </si>
+  <si>
+    <t>logoCliente</t>
+  </si>
+  <si>
+    <t>https://www.ivelpink.cl/logo-ivelpink-correo.png</t>
+  </si>
+  <si>
+    <t>https://sifg.cl/logo-sifg-correo.png</t>
+  </si>
+  <si>
+    <t>https://masautomatizacion.cl/logo-masautomatizacion.jpg</t>
+  </si>
+  <si>
+    <t>https://ingsnt.cl/logo-ingsnt-correo-white.webp</t>
   </si>
 </sst>
 </file>
@@ -492,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9B6F27-5EFA-4ABC-AF87-8DE32F38EB28}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,9 +523,10 @@
     <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="11" max="11" width="50.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -541,8 +557,11 @@
       <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -571,8 +590,11 @@
       <c r="J2">
         <v>1</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -601,8 +623,11 @@
       <c r="J3">
         <v>1</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -631,8 +656,11 @@
       <c r="J4">
         <v>1</v>
       </c>
+      <c r="K4" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -661,14 +689,17 @@
       <c r="J5">
         <v>1</v>
       </c>
+      <c r="K5" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E8" s="7"/>
     </row>
   </sheetData>
@@ -685,6 +716,10 @@
     <hyperlink ref="F5" r:id="rId10" display="mailto:Sntcontactos@gmail.com" xr:uid="{8FF307E5-8E1B-419E-A898-E141CA46693F}"/>
     <hyperlink ref="F3" r:id="rId11" display="https://mail.google.com/mail/?view=cm&amp;to=aguilera.matias.salinas@gmail.com" xr:uid="{1DA0337A-3992-4EBC-8282-C04D2DFA5384}"/>
     <hyperlink ref="F4" r:id="rId12" display="https://mail.google.com/mail/?view=cm&amp;to=aguilera.matias.salinas@gmail.com" xr:uid="{D76FD511-7009-4350-BA88-FF12C9085422}"/>
+    <hyperlink ref="K3" r:id="rId13" xr:uid="{D8963E26-AFA0-4EB1-B3A0-CC0A9451E838}"/>
+    <hyperlink ref="K2" r:id="rId14" xr:uid="{572F70D8-445F-4D7C-B602-FF9C6AC83A8F}"/>
+    <hyperlink ref="K4" r:id="rId15" xr:uid="{2D2540DC-1105-4C63-AB0A-F3EC366619B0}"/>
+    <hyperlink ref="K5" r:id="rId16" xr:uid="{1CB4C842-7D73-4709-A753-07DD41117918}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CRUD TRABAJOS + CORREO + NUEVOS CAMPOS
</commit_message>
<xml_diff>
--- a/public/database/Clientes.xlsx
+++ b/public/database/Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ignacio Aguilera\Desktop\Trabajo (SPA)\ProyectoReact\public\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3DF677-78A9-478E-9BBF-9ED678D51996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42029AA-325E-4E84-9F3D-36172786CFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,7 +148,7 @@
     <t>ag.investigadoresprivados@gmail.com</t>
   </si>
   <si>
-    <t>https://investigadores-privados.cl/logo-investigadores.jpg</t>
+    <t>https://investigadores-privados.cl/logo-investigaciones-1.png</t>
   </si>
 </sst>
 </file>
@@ -552,11 +552,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.09765625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.296875" bestFit="1" customWidth="1"/>
@@ -569,7 +569,7 @@
     <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -604,7 +604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -639,7 +639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -674,7 +674,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -709,7 +709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -744,7 +744,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -779,7 +779,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -817,8 +817,8 @@
   </sheetData>
   <autoFilter ref="A1:K1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="K7" r:id="rId1" xr:uid="{E85EC306-C209-4A28-8E14-C398A4AD483F}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{8D3D9A9A-08AD-419A-9244-CCF4EBAD9106}"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{8D3D9A9A-08AD-419A-9244-CCF4EBAD9106}"/>
+    <hyperlink ref="K7" r:id="rId2" xr:uid="{E85EC306-C209-4A28-8E14-C398A4AD483F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>